<commit_message>
Added IRIS and CAR definitive results.
</commit_message>
<xml_diff>
--- a/results/classification/car/executions_results_partial.xlsx
+++ b/results/classification/car/executions_results_partial.xlsx
@@ -12,18 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>architecture</t>
   </si>
   <si>
-    <t>acc_train</t>
-  </si>
-  <si>
-    <t>acc_validation</t>
-  </si>
-  <si>
-    <t>acc_test</t>
+    <t>partial_acc_train</t>
+  </si>
+  <si>
+    <t>partial_acc_validation</t>
+  </si>
+  <si>
+    <t>partial_acc_test</t>
+  </si>
+  <si>
+    <t>total_acc_train</t>
+  </si>
+  <si>
+    <t>total_acc_validation</t>
+  </si>
+  <si>
+    <t>total_acc_test</t>
   </si>
   <si>
     <t>percentage</t>
@@ -101,76 +110,76 @@
     <t>24</t>
   </si>
   <si>
-    <t>nnnnnnnnnnnnnnnn/nnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnnnn/nnnnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nn/nn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnn/nnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/n/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nn/nnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnn/nnn/nnn/nnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnn/nn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnn/nnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnn/nnnn/nnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnn/n/nnnnnn/nnnnnn/n/nnnnnn/nnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnn/nnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnn/nnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnn/nnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnn/nnnnnnn/nnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnnnnn/nnnn</t>
-  </si>
-  <si>
-    <t>nnnnnnnnnnnnnnnn/nnnnnnnnnnnnn/nnnn</t>
+    <t>nnnnnnnnnnnnnnnn_nnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnnnn_nnnnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nn_nn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnn_nnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_n_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nn_nnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnn_nnn_nnn_nnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnn_nn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnn_nnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnn_nnnn_nnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnn_n_nnnnnn_nnnnnn_n_nnnnnn_nnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnn_nnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnn_nnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnn_nnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnn_nnnnnnn_nnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnnnnn_nnnn</t>
+  </si>
+  <si>
+    <t>nnnnnnnnnnnnnnnn_nnnnnnnnnnnnn_nnnn</t>
   </si>
 </sst>
 </file>
@@ -238,13 +247,22 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" t="n">
         <v>0.7346891983631454</v>
@@ -256,15 +274,24 @@
         <v>0.6983709947034301</v>
       </c>
       <c r="F2" t="n">
+        <v>0.9052592035973547</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9225296440803015</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.899106674236933</v>
+      </c>
+      <c r="I2" t="n">
         <v>13.75</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" t="n">
         <v>0.7379004538209625</v>
@@ -276,15 +303,24 @@
         <v>0.7151865490912389</v>
       </c>
       <c r="F3" t="n">
+        <v>0.9605559728631035</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.957839261024837</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.9306358383068961</v>
+      </c>
+      <c r="I3" t="n">
         <v>13.75</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C4" t="n">
         <v>0.7334735036146952</v>
@@ -296,15 +332,24 @@
         <v>0.7005780361980372</v>
       </c>
       <c r="F4" t="n">
+        <v>0.9273553717037863</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9356521724790767</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.9104046245875386</v>
+      </c>
+      <c r="I4" t="n">
         <v>12.5</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C5" t="n">
         <v>0.7582001677975121</v>
@@ -316,15 +361,24 @@
         <v>0.7410404634613522</v>
       </c>
       <c r="F5" t="n">
+        <v>0.983388429702806</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9715942019310551</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9473988439995429</v>
+      </c>
+      <c r="I5" t="n">
         <v>12.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C6" t="n">
         <v>0.7207737626115716</v>
@@ -336,15 +390,24 @@
         <v>0.6888246644209346</v>
       </c>
       <c r="F6" t="n">
+        <v>0.8775482093335512</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.8999999991937536</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8766859349487834</v>
+      </c>
+      <c r="I6" t="n">
         <v>7.5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C7" t="n">
         <v>0.743902442007129</v>
@@ -356,15 +419,24 @@
         <v>0.7283237007426848</v>
       </c>
       <c r="F7" t="n">
+        <v>0.9818181814241015</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9787439603160545</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.9556840077071291</v>
+      </c>
+      <c r="I7" t="n">
         <v>7.5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C8" t="n">
         <v>0.749369217529329</v>
@@ -376,15 +448,24 @@
         <v>0.7398843941833242</v>
       </c>
       <c r="F8" t="n">
+        <v>0.9749999997044398</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.9710144911987194</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9450867052884461</v>
+      </c>
+      <c r="I8" t="n">
         <v>5.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C9" t="n">
         <v>0.7611438176830443</v>
@@ -396,15 +477,24 @@
         <v>0.7533718702421023</v>
       </c>
       <c r="F9" t="n">
+        <v>0.9834710741831252</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.977777776222874</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.9595375722543352</v>
+      </c>
+      <c r="I9" t="n">
         <v>3.75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C10" t="n">
         <v>0.7359125380058866</v>
@@ -416,15 +506,24 @@
         <v>0.6936416200475197</v>
       </c>
       <c r="F10" t="n">
+        <v>0.8904958675715549</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9043478257414224</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.8901734110936954</v>
+      </c>
+      <c r="I10" t="n">
         <v>2.5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" t="n">
         <v>0.7241379339670915</v>
@@ -436,15 +535,24 @@
         <v>0.7023121402787336</v>
       </c>
       <c r="F11" t="n">
+        <v>0.9268595042800115</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9333333331605662</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.8872832373387551</v>
+      </c>
+      <c r="I11" t="n">
         <v>2.5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C12" t="n">
         <v>0.7485281775687501</v>
@@ -456,15 +564,24 @@
         <v>0.7283237009723751</v>
       </c>
       <c r="F12" t="n">
+        <v>0.9909090906135307</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9768115940301314</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9566473990161983</v>
+      </c>
+      <c r="I12" t="n">
         <v>2.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C13" t="n">
         <v>0.7443229665868517</v>
@@ -476,15 +593,24 @@
         <v>0.716763007158489</v>
       </c>
       <c r="F13" t="n">
+        <v>0.8479338839034404</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.8898550736731378</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.8612716773341846</v>
+      </c>
+      <c r="I13" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C14" t="n">
         <v>0.7342304305633244</v>
@@ -496,15 +622,24 @@
         <v>0.6763005797573597</v>
       </c>
       <c r="F14" t="n">
+        <v>0.9074380166274457</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9101449287456015</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9017341047353138</v>
+      </c>
+      <c r="I14" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C15" t="n">
         <v>0.72750210025112</v>
@@ -516,15 +651,24 @@
         <v>0.693641620564323</v>
       </c>
       <c r="F15" t="n">
+        <v>0.8917355373871227</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0.9188405793646107</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.8901734110936953</v>
+      </c>
+      <c r="I15" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C16" t="n">
         <v>0.7199327072443533</v>
@@ -536,15 +680,24 @@
         <v>0.7052023142059415</v>
       </c>
       <c r="F16" t="n">
+        <v>0.8462809921296175</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.8782608676647794</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.8554913301688398</v>
+      </c>
+      <c r="I16" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" t="n">
         <v>0.7317073171233008</v>
@@ -556,15 +709,24 @@
         <v>0.6705202329365504</v>
       </c>
       <c r="F17" t="n">
+        <v>0.9330578514367096</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.9275362330934276</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.9190751448532061</v>
+      </c>
+      <c r="I17" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C18" t="n">
         <v>0.7300252374026633</v>
@@ -576,15 +738,24 @@
         <v>0.7052023135168703</v>
       </c>
       <c r="F18" t="n">
+        <v>0.9421487604290986</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.9507246361262557</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.9132947980323968</v>
+      </c>
+      <c r="I18" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C19" t="n">
         <v>0.742640861249752</v>
@@ -596,15 +767,24 @@
         <v>0.7167630068139533</v>
       </c>
       <c r="F19" t="n">
+        <v>0.9859504126320201</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.9739130419233571</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.9710982658959537</v>
+      </c>
+      <c r="I19" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C20" t="n">
         <v>0.7325483633752026</v>
@@ -616,15 +796,24 @@
         <v>0.705202313861406</v>
       </c>
       <c r="F20" t="n">
+        <v>0.9710743795741689</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.9739130419233571</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.9190751445086706</v>
+      </c>
+      <c r="I20" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C21" t="n">
         <v>0.7350715005267459</v>
@@ -636,15 +825,24 @@
         <v>0.7109826603376797</v>
       </c>
       <c r="F21" t="n">
+        <v>0.9801652892561984</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.9768115926479948</v>
+      </c>
+      <c r="H21" t="n">
+        <v>0.942196532136443</v>
+      </c>
+      <c r="I21" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C22" t="n">
         <v>0.75777965087265</v>
@@ -656,15 +854,24 @@
         <v>0.7456647412625351</v>
       </c>
       <c r="F22" t="n">
+        <v>0.9925619834710744</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.9797101433726324</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0.976878612716763</v>
+      </c>
+      <c r="I22" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C23" t="n">
         <v>0.8031959577805862</v>
@@ -676,15 +883,24 @@
         <v>0.7861271686636644</v>
       </c>
       <c r="F23" t="n">
+        <v>0.9933884297520661</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0.9739130419233571</v>
+      </c>
+      <c r="H23" t="n">
+        <v>0.9884393063583815</v>
+      </c>
+      <c r="I23" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C24" t="n">
         <v>0.7586206862964582</v>
@@ -696,15 +912,24 @@
         <v>0.7572254342150826</v>
       </c>
       <c r="F24" t="n">
+        <v>0.9694214877018259</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.9623188390248064</v>
+      </c>
+      <c r="H24" t="n">
+        <v>0.9364161849710982</v>
+      </c>
+      <c r="I24" t="n">
         <v>1.25</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C25" t="n">
         <v>0.7939444914196999</v>
@@ -716,6 +941,15 @@
         <v>0.7803468221873906</v>
       </c>
       <c r="F25" t="n">
+        <v>0.9991735537190083</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.9855072448219078</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.9826589595375722</v>
+      </c>
+      <c r="I25" t="n">
         <v>1.25</v>
       </c>
     </row>

</xml_diff>